<commit_message>
Se soluciono la seleccion de facturas en SAP
</commit_message>
<xml_diff>
--- a/Proceso1_Lala/Data/Output/Incidents.xlsx
+++ b/Proceso1_Lala/Data/Output/Incidents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\cruzl\Documents\Proyecto\LALA\Proceso1_Lala\Data\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C624D40-3A0B-4AF6-8F73-686DB1A0389E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452C2379-AA4F-470C-8A0F-C6563E37318D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{CD3CAB56-BE71-4485-8FBE-BEAF51E98128}"/>
   </bookViews>
@@ -417,7 +417,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection sqref="A1 A1 A1:C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
-Busqueda y descarga de facturas en intranet (Falta retenciones y agregar excepcion si no hay factura en intranet)
</commit_message>
<xml_diff>
--- a/Proceso1_Lala/Data/Output/Incidents.xlsx
+++ b/Proceso1_Lala/Data/Output/Incidents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\cruzl\Documents\Proyecto\LALA\Proceso1_Lala\Data\Output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\cruzl\Documents\UiPath\Proceso1_Lala\Proceso1_Lala\Data\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452C2379-AA4F-470C-8A0F-C6563E37318D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07F74C6-BBA6-45F4-91EC-1FE3E5421122}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{CD3CAB56-BE71-4485-8FBE-BEAF51E98128}"/>
+    <workbookView xWindow="23880" yWindow="780" windowWidth="20730" windowHeight="11310" xr2:uid="{CD3CAB56-BE71-4485-8FBE-BEAF51E98128}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -417,7 +417,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection sqref="A1 A1 A1:C1"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se agrego modulo para agregar comentario en caso de que falle
</commit_message>
<xml_diff>
--- a/Proceso1_Lala/Data/Output/Incidents.xlsx
+++ b/Proceso1_Lala/Data/Output/Incidents.xlsx
@@ -5,12 +5,12 @@
   <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\cruzl\Documents\UiPath\Proyecto\Proceso1_Lala\Data\Output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\cruzl\Desktop\LALA\Proceso1_Lala\Data\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A204EC18-B029-4E34-96B1-A488CA0C40A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9D2D0D-0872-41D1-BA10-9DF57B626B31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="1800" yWindow="3870" windowWidth="18000" windowHeight="9480" firstSheet="0" activeTab="0" xr2:uid="{CD3CAB56-BE71-4485-8FBE-BEAF51E98128}"/>
+    <x:workbookView xWindow="-120" yWindow="330" windowWidth="24240" windowHeight="13290" firstSheet="0" activeTab="0" xr2:uid="{CD3CAB56-BE71-4485-8FBE-BEAF51E98128}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <x:si>
     <x:t>UUID Invoce</x:t>
   </x:si>
@@ -37,16 +37,13 @@
     <x:t>Posible Mistake</x:t>
   </x:si>
   <x:si>
-    <x:t>E561D9BE-1510-4A73-B36A-D78A58728837</x:t>
+    <x:t>2FBB1D0A-DC81-4451-8C7C-D5A00E9F1168</x:t>
   </x:si>
   <x:si>
-    <x:t>12/21/2020 16:22:07</x:t>
+    <x:t>12/22/2020 17:57:47</x:t>
   </x:si>
   <x:si>
     <x:t>- Error F5061</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12/21/2020 16:40:29</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -116,7 +113,7 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="9">
+  <x:cellStyleXfs count="7">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
@@ -131,12 +128,6 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="22" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -532,15 +523,8 @@
       </x:c>
     </x:row>
     <x:row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="10" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="B3" s="11" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C3" s="7" t="s">
-        <x:v>5</x:v>
-      </x:c>
+      <x:c r="A3" s="10" t="s"/>
+      <x:c r="B3" s="11" t="s"/>
     </x:row>
     <x:row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A4" s="10" t="s"/>
@@ -551,7 +535,7 @@
       <x:c r="B5" s="11" t="s"/>
     </x:row>
     <x:row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <x:c r="A6" s="10" t="s"/>
+      <x:c r="A6" s="12" t="s"/>
       <x:c r="B6" s="11" t="s"/>
     </x:row>
     <x:row r="7" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Solo falta solucionar en caso de que tenga 2 posiciones o mas
</commit_message>
<xml_diff>
--- a/Proceso1_Lala/Data/Output/Incidents.xlsx
+++ b/Proceso1_Lala/Data/Output/Incidents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\cruzl\Desktop\LALA\Proceso1_Lala\Data\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BA1238-264B-4C1A-9B4D-4A9897A84D19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F9914D-FF81-4633-9B7F-D1D6D6A06916}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{CD3CAB56-BE71-4485-8FBE-BEAF51E98128}"/>
+    <workbookView xWindow="3990" yWindow="1575" windowWidth="18000" windowHeight="9480" xr2:uid="{CD3CAB56-BE71-4485-8FBE-BEAF51E98128}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -430,7 +430,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection sqref="A1 A1 A1:C1"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="A2:D4"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>